<commit_message>
add extented features to estimations
</commit_message>
<xml_diff>
--- a/assignment-2/estimation-template.xlsx
+++ b/assignment-2/estimation-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation Template" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Late Joiners</t>
   </si>
@@ -67,37 +67,13 @@
     <t xml:space="preserve">Our system should display to users the actual results for games that have concluded where that user had a pick, as well as data about their overall picking record.</t>
   </si>
   <si>
-    <t xml:space="preserve">{MVF List all others}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{MVF e.g 6 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{MVF e.g 7 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etc..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature 1 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature 2 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature 3 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All other Extended Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature e.g 4 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature e.g 5 - Insert title}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{Extended Feature e.g 6 - Insert title}</t>
+    <t xml:space="preserve">Our system should source tournament and game data in real-time from APIs for tournaments where an API is available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system should have the ability to 'crowd-source' result information. i.e. Users can enter the score for a game and once a threshold of submitted results have been submitted, the results for the game will be updated and players scored on their picks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our system should have a suitable schedule and process for automatic backups of the database. This can be integrated as part of the Heroku platform we plan to deploy on.</t>
   </si>
 </sst>
 </file>
@@ -385,15 +361,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4285714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
@@ -601,143 +577,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="11" t="e">
-        <f aca="false">AVERAGEIF(B12:G12,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="11" t="e">
-        <f aca="false">AVERAGEIF(B13:G13,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="11" t="e">
-        <f aca="false">AVERAGEIF(B14:G14,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="11" t="e">
-        <f aca="false">AVERAGEIF(B15:G15,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="11" t="e">
-        <f aca="false">AVERAGEIF(B16:G16,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="11" t="e">
-        <f aca="false">AVERAGEIF(B17:G17,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="11" t="e">
-        <f aca="false">AVERAGEIF(B18:G18,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="11" t="e">
-        <f aca="false">AVERAGEIF(B19:G19,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="11" t="e">
-        <f aca="false">AVERAGEIF(B20:G20,"&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H21" s="15" t="e">
-        <f aca="false">SUM(H4:H20)</f>
+      <c r="H12" s="15" t="e">
+        <f aca="false">SUM(H4:H11)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>